<commit_message>
actualizar git ignore y archivos de excel
</commit_message>
<xml_diff>
--- a/report/ErrorCuadMedio.xlsx
+++ b/report/ErrorCuadMedio.xlsx
@@ -105,6 +105,1202 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Error</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Cuadrático Medio por frame</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" i="1" baseline="0"/>
+              <a:t>(escena 2.2 esqueleto 9)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050" i="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Escena2.2esq9!$D$1:$D$250</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="250"/>
+                <c:pt idx="0">
+                  <c:v>3.4575691488561593E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4729194794681423E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7226958083993227E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4212815844769581E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8540789264472262E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4472092469892766E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.782193728530768E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.341722334402928E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2672084500851933E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4122270280081635E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3553397038786938E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.4091667367046989E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.3972945216941601E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.4841833511643418E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.4856625488831727E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3750644403909971E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8889740748481332E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9011455922665937E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.8320690779054624E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7526199686592321E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.7682970011616565E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.3133533988170476E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.497940969475772E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.5514862004070058E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.4873399602864619E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.4983990636391071E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.9967823835237372E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.7357688205170027E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.5317215386919558E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.4831799576077925E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.4962009329036238E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.4355594768358033E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.4883409856802952E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.5444333271529016E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.9524044163608316E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.6252763395327674E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.55636169379328E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.5299912463350888E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.549729305995223E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.5855097367772822E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.5786460007871841E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.4410005711803832E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.3687699944604521E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.3640147131564102E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.3527435529752236E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.367415435066571E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.3094541893927534E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.3243470060502531E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.3469450141756285E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.3610493088871742E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.7544403196940045E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.4381957607212257E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.4117137990145936E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.7060696619916601E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.3220787578419259E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.339341325658543E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.4740905864482988E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.4997688543715343E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.4979346946170373E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.8346499907454382E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.4890208226820707E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.3819483437232546E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.3558182596534175E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.4984229043162764E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.6457241966276158E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.5252177615706752E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.5960749276611664E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.6300366329860938E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.6082490055550566E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.5644015712028944E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.5600271125167011E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.6177501967022248E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.7176895677913928E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.676329651115158E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.5852590118806413E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.6170141498797888E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.6598780455351615E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.6207469387949665E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.8087477760919614E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.6083345202398011E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.4349781343833027E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.2641741512654624E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.0915942786113921E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.5655188998824994E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.5222150770003508E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.2338226949633746E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.8373453303005187E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.1534343838764589E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.13762480512502137</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.13938750175818748</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.14269928889029751</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.10997284392017868</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.14709003955747788</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.16494517014983989</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.17470880983388562</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.19659544931836237</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.23262102798796891</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.25180090092548063</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.27598773769063373</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.30484860177716844</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.31886462317133485</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.36784270535340896</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.38512739492263592</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.40947808499042626</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.440045667890749</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.46729723407732288</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.4751781488820318</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.50225714882701245</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.52408803647059621</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.55042841795343656</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.5857762008943509</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.61313447954008593</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.64046133286046203</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.64419411968076479</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.67623889171708773</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.70926150103751029</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.76572513418107879</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.77105939454618289</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.80292376267390264</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.8116915902720967</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.82762021333930957</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.70370442345744089</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.71176346269666224</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.71871944352974992</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.72282739083812875</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.72169637415225374</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.72744862529806753</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.73978432940667715</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.74208708708972282</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.74637192549292597</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.74461741217168209</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.78540542249405187</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.77672169899419374</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.77484757715827501</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.76513312279802748</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.72309500004510718</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.71613150605044662</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.72006062860948949</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.70258867567260519</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.69915482847321742</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.69390559791232298</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.68933702028099053</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.68656906299249931</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.68658180554870885</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.68845166742327779</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.68850842339233753</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.68746333017916406</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.6871273285814804</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.68656965001599524</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.68460305206247396</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.68304621017349632</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.6811491655442089</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.67922584559676302</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.67769957153019422</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.67691888808345635</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.67562898942507998</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.67545762906220386</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.67621760542316434</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.67635033181549897</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.67664508097504239</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.67670166907891249</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.67635929677996598</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.67705894653028453</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.67733947649399284</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.67713402841630843</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.67854759840943746</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.67887579447231083</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.67911295716507436</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.68024692231454087</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.68040160991553145</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.68134690444786317</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.68200502785563355</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.68282543582766952</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.68365950608329396</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.68512180722723826</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.68653157998552894</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.68781732723663158</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.68859708902687877</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.68943521257815676</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.68980519473233892</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.69016447687399063</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.68874888281011493</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.68836822313729706</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.68919801505040823</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.6858914863242862</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.68302394656728949</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.66876968830059558</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.6570697612498505</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.64315010310424703</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.63367851152982813</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.69595028436839923</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.70587301882082687</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.70687402175940062</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.711223137700147</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.70885872928076155</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.70773651340443766</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.70161998162735073</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.71545972253462276</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.70793136181742056</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.69853077975507338</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.67742707708637584</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.6666815073397675</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.72882474401627761</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.73357324171204452</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.73553589073044523</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.8608815942140966</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.74427285147883582</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.74976650300715253</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.7515344037014714</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.76433962818241885</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.76963060513396453</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.76554419281557973</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.77720676009908185</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.76999292230879146</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.76933954869953414</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.77730224931657366</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.76892361313013469</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.77306312150823064</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.77090588192700016</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.77131693267429002</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.77066615347407541</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.76987247337421183</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.85768606410794745</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.78880434976593305</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.63431986901572501</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.57558866740623316</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.54711026503434923</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.56523289659823883</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.55395071901756077</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.53997751524250848</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.54677514552812367</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.58505146573924749</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.58198201892471213</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.584999357243707</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.58321460278492843</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.51889312596459913</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.54617774247751338</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.58756027390986365</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.56723163404653409</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.47255750949869768</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.43363813863741535</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.41666837832202819</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.436235265084298</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.4462698466320284</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.43251175016196752</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.57317232575533394</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.42488091979452586</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.426474498954028</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.4337907468320803</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.43179843446283667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="711856864"/>
+        <c:axId val="711854688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="711856864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="711854688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="711854688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ECM</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [rad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>²</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="711856864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Erro</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>r Cuadrático Medio por frame</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" i="1" baseline="0"/>
+              <a:t>(escena corregida a mano vs )</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2129,16 +3325,72 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1019816064"/>
-        <c:axId val="-1019818240"/>
+        <c:axId val="711850880"/>
+        <c:axId val="711859040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1019816064"/>
+        <c:axId val="711850880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frames</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2175,7 +3427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1019818240"/>
+        <c:crossAx val="711859040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2183,7 +3435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1019818240"/>
+        <c:axId val="711859040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2203,6 +3455,78 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ECM</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [rad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>²</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2234,7 +3558,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1019816064"/>
+        <c:crossAx val="711850880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2284,6 +3608,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2839,25 +4203,578 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>618</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>632</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3143,8 +5060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D651"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A609" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B651" sqref="B651"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10976,11 +12893,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregando reporte final en PDF
</commit_message>
<xml_diff>
--- a/report/ErrorCuadMedio.xlsx
+++ b/report/ErrorCuadMedio.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="5" r:id="rId1"/>
@@ -183,7 +183,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1649,11 +1648,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="662257280"/>
-        <c:axId val="662249664"/>
+        <c:axId val="220487392"/>
+        <c:axId val="220491200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="662257280"/>
+        <c:axId val="220487392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,7 +1684,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1751,7 +1749,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662249664"/>
+        <c:crossAx val="220491200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1759,7 +1757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="662249664"/>
+        <c:axId val="220491200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,7 +1819,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1882,7 +1879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662257280"/>
+        <c:crossAx val="220487392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1985,6 +1982,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2039,6 +2037,7 @@
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3963,11 +3962,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="662248576"/>
-        <c:axId val="662249120"/>
+        <c:axId val="220491744"/>
+        <c:axId val="46795008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="662248576"/>
+        <c:axId val="220491744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3999,6 +3998,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4064,7 +4064,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662249120"/>
+        <c:crossAx val="46795008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4072,7 +4072,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="662249120"/>
+        <c:axId val="46795008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -4130,6 +4130,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4190,7 +4191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662248576"/>
+        <c:crossAx val="220491744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4204,6 +4205,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4328,7 +4330,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6931,11 +6932,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="662251296"/>
-        <c:axId val="662251840"/>
+        <c:axId val="270816416"/>
+        <c:axId val="270806624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="662251296"/>
+        <c:axId val="270816416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6967,7 +6968,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7033,7 +7033,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662251840"/>
+        <c:crossAx val="270806624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7041,7 +7041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="662251840"/>
+        <c:axId val="270806624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7098,7 +7098,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7159,7 +7158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662251296"/>
+        <c:crossAx val="270816416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7173,7 +7172,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10207,11 +10205,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="479962512"/>
-        <c:axId val="479965232"/>
+        <c:axId val="270816960"/>
+        <c:axId val="270804448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="479962512"/>
+        <c:axId val="270816960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10309,7 +10307,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479965232"/>
+        <c:crossAx val="270804448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10317,7 +10315,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479965232"/>
+        <c:axId val="270804448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10435,7 +10433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479962512"/>
+        <c:crossAx val="270816960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10632,6 +10630,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -13486,11 +13485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="719896000"/>
-        <c:axId val="719892192"/>
+        <c:axId val="270803360"/>
+        <c:axId val="270815872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="719896000"/>
+        <c:axId val="270803360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13588,7 +13587,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="719892192"/>
+        <c:crossAx val="270815872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13596,7 +13595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="719892192"/>
+        <c:axId val="270815872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13714,7 +13713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="719896000"/>
+        <c:crossAx val="270803360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27276,8 +27275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C421"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33455,7 +33454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -37203,8 +37202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B466"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
agregar ultima version del PDF para impresión y presentación
</commit_message>
<xml_diff>
--- a/report/ErrorCuadMedio.xlsx
+++ b/report/ErrorCuadMedio.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>original vs glitches</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Original vs corregido</t>
+  </si>
+  <si>
+    <t>Ground Truth vs glitched</t>
+  </si>
+  <si>
+    <t>Ground Truth vs corregido</t>
   </si>
 </sst>
 </file>
@@ -1648,11 +1654,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="220487392"/>
-        <c:axId val="220491200"/>
+        <c:axId val="-1856953952"/>
+        <c:axId val="-1856951776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="220487392"/>
+        <c:axId val="-1856953952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,7 +1755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220491200"/>
+        <c:crossAx val="-1856951776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1757,7 +1763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220491200"/>
+        <c:axId val="-1856951776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,7 +1885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220487392"/>
+        <c:crossAx val="-1856953952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2027,7 +2033,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>original vs glitches</c:v>
+                  <c:v>Ground Truth vs glitched</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2995,7 +3001,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>original vs corregido</c:v>
+                  <c:v>Ground Truth vs corregido</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3962,11 +3968,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="220491744"/>
-        <c:axId val="46795008"/>
+        <c:axId val="-1856949056"/>
+        <c:axId val="-1856945248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="220491744"/>
+        <c:axId val="-1856949056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4064,7 +4070,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46795008"/>
+        <c:crossAx val="-1856945248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4072,7 +4078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46795008"/>
+        <c:axId val="-1856945248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -4191,7 +4197,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220491744"/>
+        <c:crossAx val="-1856949056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6932,11 +6938,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="270816416"/>
-        <c:axId val="270806624"/>
+        <c:axId val="-1856946880"/>
+        <c:axId val="-1856947424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="270816416"/>
+        <c:axId val="-1856946880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7033,7 +7039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270806624"/>
+        <c:crossAx val="-1856947424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7041,7 +7047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="270806624"/>
+        <c:axId val="-1856947424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7158,7 +7164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270816416"/>
+        <c:crossAx val="-1856946880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7296,7 +7302,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10205,11 +10210,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="270816960"/>
-        <c:axId val="270804448"/>
+        <c:axId val="-1856938720"/>
+        <c:axId val="-1856944704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="270816960"/>
+        <c:axId val="-1856938720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10241,7 +10246,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10307,7 +10311,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270804448"/>
+        <c:crossAx val="-1856944704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10315,7 +10319,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="270804448"/>
+        <c:axId val="-1856944704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10372,7 +10376,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10433,7 +10436,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270816960"/>
+        <c:crossAx val="-1856938720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10447,7 +10450,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10620,7 +10622,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Original vs glitched</c:v>
+                  <c:v>Ground Truth vs glitched</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12053,7 +12055,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Original vs corregido</c:v>
+                  <c:v>Ground Truth vs corregido</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12063,6 +12065,7 @@
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -13485,11 +13488,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="270803360"/>
-        <c:axId val="270815872"/>
+        <c:axId val="-1856943616"/>
+        <c:axId val="-1856943072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="270803360"/>
+        <c:axId val="-1856943616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13587,7 +13590,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270815872"/>
+        <c:crossAx val="-1856943072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13595,7 +13598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="270815872"/>
+        <c:axId val="-1856943072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13713,7 +13716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270803360"/>
+        <c:crossAx val="-1856943616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27275,22 +27278,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C421"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -37203,21 +37207,21 @@
   <dimension ref="A1:B466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>